<commit_message>
Allen Richy - 4/26/2021 - NHOP and VOIP
</commit_message>
<xml_diff>
--- a/Configration/GEP_Bot_Configuration_File.xlsx
+++ b/Configration/GEP_Bot_Configuration_File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gep1-my.sharepoint.com/personal/allen_richy_gep_com/Documents/GEP Automation/Configration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="168" documentId="13_ncr:1_{6EA17F22-868C-46CD-8BBC-388BA0C82BDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B7FB747C-40DF-40E6-BCFA-C88204D83536}"/>
+  <xr:revisionPtr revIDLastSave="169" documentId="13_ncr:1_{6EA17F22-868C-46CD-8BBC-388BA0C82BDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E1398FE4-1AA1-445B-970F-52FE9A5463CE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_SPOC_NHOP_Confirmation" sheetId="1" r:id="rId1"/>
@@ -360,9 +360,6 @@
     <t>NHOP O365 Team Licence, MFA Failure Templete</t>
   </si>
   <si>
-    <t>Any where in between execution of NHOP O365 Team Licence, MFA</t>
-  </si>
-  <si>
     <t>NHOP User Joining Confirmation Failure Templete</t>
   </si>
   <si>
@@ -815,6 +812,9 @@
   </si>
   <si>
     <t>Country_LWD_Time</t>
+  </si>
+  <si>
+    <t>Any where in between execution of NHOP O365 Team Licence, MFA, VOIP</t>
   </si>
 </sst>
 </file>
@@ -1565,7 +1565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1588,7 +1588,7 @@
         <v>45</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1602,7 +1602,7 @@
         <v>46</v>
       </c>
       <c r="D2" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E2" s="9">
         <v>0.79166666666666663</v>
@@ -1623,7 +1623,7 @@
         <v>48</v>
       </c>
       <c r="D3" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E3" s="11">
         <v>0.79166666666666663</v>
@@ -1643,7 +1643,7 @@
         <v>48</v>
       </c>
       <c r="D4" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E4" s="11">
         <v>0.79166666666666663</v>
@@ -1663,7 +1663,7 @@
         <v>47</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E5" s="11">
         <v>0.79166666666666663</v>
@@ -1683,7 +1683,7 @@
         <v>47</v>
       </c>
       <c r="D6" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E6" s="16">
         <v>0.79166666666666663</v>
@@ -1703,7 +1703,7 @@
         <v>49</v>
       </c>
       <c r="D7" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E7" s="20">
         <v>0.41666666666666669</v>
@@ -1723,7 +1723,7 @@
         <v>50</v>
       </c>
       <c r="D8" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E8" s="9">
         <v>0.29166666666666669</v>
@@ -1743,7 +1743,7 @@
         <v>50</v>
       </c>
       <c r="D9" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E9" s="11">
         <v>0.29166666666666669</v>
@@ -1763,7 +1763,7 @@
         <v>50</v>
       </c>
       <c r="D10" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E10" s="11">
         <v>0.29166666666666669</v>
@@ -1783,7 +1783,7 @@
         <v>51</v>
       </c>
       <c r="D11" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E11" s="11">
         <v>0.29166666666666669</v>
@@ -1803,7 +1803,7 @@
         <v>51</v>
       </c>
       <c r="D12" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E12" s="11">
         <v>0.29166666666666669</v>
@@ -1823,7 +1823,7 @@
         <v>51</v>
       </c>
       <c r="D13" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E13" s="11">
         <v>0.29166666666666669</v>
@@ -1843,7 +1843,7 @@
         <v>51</v>
       </c>
       <c r="D14" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E14" s="11">
         <v>0.29166666666666669</v>
@@ -1863,7 +1863,7 @@
         <v>51</v>
       </c>
       <c r="D15" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E15" s="16">
         <v>0.29166666666666669</v>
@@ -1883,7 +1883,7 @@
         <v>52</v>
       </c>
       <c r="D16" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E16" s="9">
         <v>0.29166666666666669</v>
@@ -1903,7 +1903,7 @@
         <v>52</v>
       </c>
       <c r="D17" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E17" s="11">
         <v>0.58333333333333337</v>
@@ -1923,7 +1923,7 @@
         <v>49</v>
       </c>
       <c r="D18" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E18" s="24">
         <v>0.45833333333333331</v>
@@ -1943,7 +1943,7 @@
         <v>48</v>
       </c>
       <c r="D19" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E19" s="9">
         <v>0.58333333333333337</v>
@@ -1963,7 +1963,7 @@
         <v>48</v>
       </c>
       <c r="D20" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E20" s="11">
         <v>0.58333333333333337</v>
@@ -1983,7 +1983,7 @@
         <v>48</v>
       </c>
       <c r="D21" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E21" s="11">
         <v>0.58333333333333337</v>
@@ -2003,7 +2003,7 @@
         <v>48</v>
       </c>
       <c r="D22" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E22" s="11">
         <v>0.58333333333333337</v>
@@ -2023,7 +2023,7 @@
         <v>48</v>
       </c>
       <c r="D23" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E23" s="11">
         <v>0.58333333333333337</v>
@@ -2043,7 +2043,7 @@
         <v>48</v>
       </c>
       <c r="D24" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E24" s="11">
         <v>0.58333333333333337</v>
@@ -2063,7 +2063,7 @@
         <v>48</v>
       </c>
       <c r="D25" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E25" s="11">
         <v>0.58333333333333337</v>
@@ -2083,7 +2083,7 @@
         <v>48</v>
       </c>
       <c r="D26" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E26" s="11">
         <v>0.58333333333333337</v>
@@ -2103,7 +2103,7 @@
         <v>48</v>
       </c>
       <c r="D27" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E27" s="11">
         <v>0.58333333333333337</v>
@@ -2123,7 +2123,7 @@
         <v>48</v>
       </c>
       <c r="D28" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E28" s="11">
         <v>0.58333333333333337</v>
@@ -2143,7 +2143,7 @@
         <v>48</v>
       </c>
       <c r="D29" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E29" s="11">
         <v>0.58333333333333337</v>
@@ -2163,7 +2163,7 @@
         <v>48</v>
       </c>
       <c r="D30" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E30" s="11">
         <v>0.58333333333333337</v>
@@ -2183,7 +2183,7 @@
         <v>48</v>
       </c>
       <c r="D31" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E31" s="11">
         <v>0.58333333333333337</v>
@@ -2203,7 +2203,7 @@
         <v>48</v>
       </c>
       <c r="D32" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E32" s="11">
         <v>0.58333333333333337</v>
@@ -2223,7 +2223,7 @@
         <v>53</v>
       </c>
       <c r="D33" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E33" s="11">
         <v>0.58333333333333337</v>
@@ -2243,7 +2243,7 @@
         <v>54</v>
       </c>
       <c r="D34" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E34" s="16">
         <v>0.58333333333333337</v>
@@ -2263,7 +2263,7 @@
         <v>55</v>
       </c>
       <c r="D35" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E35" s="9">
         <v>0.79166666666666663</v>
@@ -2283,7 +2283,7 @@
         <v>55</v>
       </c>
       <c r="D36" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E36" s="16">
         <v>0.79166666666666663</v>
@@ -2324,20 +2324,20 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4">
         <v>123456</v>
@@ -2345,32 +2345,32 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2382,9 +2382,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F323925-C95A-4104-A479-BD78924E652C}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2411,13 +2411,13 @@
         <v>58</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>59</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E1" s="31" t="s">
         <v>60</v>
@@ -2438,13 +2438,13 @@
         <v>65</v>
       </c>
       <c r="K1" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="L1" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="M1" s="32" t="s">
         <v>140</v>
-      </c>
-      <c r="M1" s="32" t="s">
-        <v>141</v>
       </c>
       <c r="N1"/>
     </row>
@@ -2453,40 +2453,40 @@
         <v>1</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C2" s="28" t="s">
         <v>66</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E2" s="28" t="s">
         <v>67</v>
       </c>
       <c r="F2" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="G2" s="43" t="s">
         <v>183</v>
-      </c>
-      <c r="G2" s="43" t="s">
-        <v>184</v>
       </c>
       <c r="H2" s="28" t="s">
         <v>68</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J2" s="45" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K2" s="33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L2" s="33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M2" s="33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N2"/>
     </row>
@@ -2495,40 +2495,40 @@
         <v>2</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>69</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E3" s="25" t="s">
         <v>70</v>
       </c>
       <c r="F3" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="G3" s="43" t="s">
         <v>183</v>
-      </c>
-      <c r="G3" s="43" t="s">
-        <v>184</v>
       </c>
       <c r="H3" s="25" t="s">
         <v>68</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J3" s="41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K3" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="L3" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="L3" s="34" t="s">
-        <v>146</v>
-      </c>
       <c r="M3" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N3"/>
     </row>
@@ -2537,43 +2537,43 @@
         <v>3</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>71</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E4" s="25" t="s">
         <v>72</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G4" s="43" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H4" s="25" t="s">
         <v>73</v>
       </c>
       <c r="I4" s="25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J4" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="K4" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="L4" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="M4" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="N4" s="37" t="s">
         <v>149</v>
-      </c>
-      <c r="K4" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="L4" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="M4" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="N4" s="37" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -2581,22 +2581,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>71</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E5" s="25" t="s">
         <v>75</v>
       </c>
       <c r="F5" s="35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G5" s="43" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H5" s="25" t="s">
         <v>73</v>
@@ -2605,16 +2605,16 @@
         <v>74</v>
       </c>
       <c r="J5" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="K5" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="K5" s="34" t="s">
+      <c r="L5" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="L5" s="34" t="s">
+      <c r="M5" s="38" t="s">
         <v>154</v>
-      </c>
-      <c r="M5" s="38" t="s">
-        <v>155</v>
       </c>
       <c r="N5"/>
     </row>
@@ -2623,22 +2623,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>71</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E6" s="25" t="s">
         <v>76</v>
       </c>
       <c r="F6" s="35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G6" s="43" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H6" s="25" t="s">
         <v>73</v>
@@ -2647,16 +2647,16 @@
         <v>74</v>
       </c>
       <c r="J6" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="K6" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="K6" s="34" t="s">
+      <c r="L6" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="L6" s="34" t="s">
+      <c r="M6" s="38" t="s">
         <v>154</v>
-      </c>
-      <c r="M6" s="38" t="s">
-        <v>155</v>
       </c>
       <c r="N6"/>
     </row>
@@ -2665,40 +2665,40 @@
         <v>6</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>77</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E7" s="25" t="s">
         <v>78</v>
       </c>
       <c r="F7" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="G7" s="43" t="s">
         <v>183</v>
-      </c>
-      <c r="G7" s="43" t="s">
-        <v>184</v>
       </c>
       <c r="H7" s="25" t="s">
         <v>68</v>
       </c>
       <c r="I7" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J7" s="41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K7" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L7" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M7" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N7"/>
     </row>
@@ -2707,40 +2707,40 @@
         <v>7</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>79</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E8" s="25" t="s">
         <v>80</v>
       </c>
       <c r="F8" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="G8" s="43" t="s">
         <v>183</v>
-      </c>
-      <c r="G8" s="43" t="s">
-        <v>184</v>
       </c>
       <c r="H8" s="25" t="s">
         <v>81</v>
       </c>
       <c r="I8" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="J8" s="44" t="s">
         <v>210</v>
       </c>
-      <c r="J8" s="44" t="s">
-        <v>211</v>
-      </c>
       <c r="K8" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L8" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M8" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N8"/>
     </row>
@@ -2749,40 +2749,40 @@
         <v>8</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>82</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E9" s="25" t="s">
         <v>83</v>
       </c>
       <c r="F9" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="G9" s="43" t="s">
         <v>183</v>
-      </c>
-      <c r="G9" s="43" t="s">
-        <v>184</v>
       </c>
       <c r="H9" s="25" t="s">
         <v>81</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J9" s="44" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K9" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L9" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M9" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N9"/>
     </row>
@@ -2791,40 +2791,40 @@
         <v>9</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>84</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E10" s="25" t="s">
         <v>85</v>
       </c>
       <c r="F10" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="G10" s="43" t="s">
         <v>183</v>
-      </c>
-      <c r="G10" s="43" t="s">
-        <v>184</v>
       </c>
       <c r="H10" s="25" t="s">
         <v>68</v>
       </c>
       <c r="I10" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J10" s="41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K10" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L10" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M10" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N10"/>
     </row>
@@ -2833,40 +2833,40 @@
         <v>10</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>86</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>87</v>
+        <v>216</v>
       </c>
       <c r="F11" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="G11" s="43" t="s">
         <v>183</v>
-      </c>
-      <c r="G11" s="43" t="s">
-        <v>184</v>
       </c>
       <c r="H11" s="25" t="s">
         <v>68</v>
       </c>
       <c r="I11" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J11" s="41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K11" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L11" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M11" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N11"/>
     </row>
@@ -2875,40 +2875,40 @@
         <v>11</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C12" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="E12" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D12" s="28" t="s">
-        <v>162</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>89</v>
-      </c>
       <c r="F12" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="G12" s="43" t="s">
         <v>183</v>
-      </c>
-      <c r="G12" s="43" t="s">
-        <v>184</v>
       </c>
       <c r="H12" s="25" t="s">
         <v>68</v>
       </c>
       <c r="I12" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J12" s="41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K12" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L12" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M12" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N12"/>
     </row>
@@ -2917,43 +2917,43 @@
         <v>12</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C13" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="E13" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="F13" s="35" t="s">
         <v>163</v>
       </c>
-      <c r="E13" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="F13" s="35" t="s">
-        <v>164</v>
-      </c>
       <c r="G13" s="43" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H13" s="25" t="s">
         <v>73</v>
       </c>
       <c r="I13" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J13" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="K13" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="L13" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="K13" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="L13" s="34" t="s">
+      <c r="M13" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="M13" s="38" t="s">
+      <c r="N13" s="37" t="s">
         <v>167</v>
-      </c>
-      <c r="N13" s="37" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="87" x14ac:dyDescent="0.35">
@@ -2961,40 +2961,40 @@
         <v>13</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C14" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="E14" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="D14" s="28" t="s">
-        <v>169</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>93</v>
-      </c>
       <c r="F14" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="G14" s="43" t="s">
         <v>183</v>
-      </c>
-      <c r="G14" s="43" t="s">
-        <v>184</v>
       </c>
       <c r="H14" s="25" t="s">
         <v>68</v>
       </c>
       <c r="I14" s="25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J14" s="41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K14" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L14" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M14" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N14"/>
     </row>
@@ -3003,40 +3003,40 @@
         <v>14</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C15" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="E15" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="28" t="s">
-        <v>170</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>95</v>
-      </c>
       <c r="F15" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="G15" s="43" t="s">
         <v>183</v>
-      </c>
-      <c r="G15" s="43" t="s">
-        <v>184</v>
       </c>
       <c r="H15" s="25" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J15" s="44" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K15" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L15" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M15" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N15"/>
     </row>
@@ -3045,40 +3045,40 @@
         <v>15</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C16" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="E16" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="D16" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>98</v>
-      </c>
       <c r="F16" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="G16" s="43" t="s">
         <v>183</v>
-      </c>
-      <c r="G16" s="43" t="s">
-        <v>184</v>
       </c>
       <c r="H16" s="25" t="s">
         <v>68</v>
       </c>
       <c r="I16" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J16" s="41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K16" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L16" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M16" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N16"/>
     </row>
@@ -3087,40 +3087,40 @@
         <v>16</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C17" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="E17" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="D17" s="28" t="s">
-        <v>172</v>
-      </c>
-      <c r="E17" s="25" t="s">
-        <v>100</v>
-      </c>
       <c r="F17" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="G17" s="43" t="s">
         <v>183</v>
-      </c>
-      <c r="G17" s="43" t="s">
-        <v>184</v>
       </c>
       <c r="H17" s="25" t="s">
         <v>68</v>
       </c>
       <c r="I17" s="25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J17" s="41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K17" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L17" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M17" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N17"/>
     </row>
@@ -3129,40 +3129,40 @@
         <v>17</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C18" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="E18" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="28" t="s">
-        <v>173</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>102</v>
-      </c>
       <c r="F18" s="35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G18" s="43" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H18" s="25" t="s">
         <v>73</v>
       </c>
       <c r="I18" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J18" s="42" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K18" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L18" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M18" s="38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N18"/>
     </row>
@@ -3171,40 +3171,40 @@
         <v>18</v>
       </c>
       <c r="B19" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="D19" s="28" t="s">
         <v>199</v>
       </c>
-      <c r="C19" s="25" t="s">
-        <v>198</v>
-      </c>
-      <c r="D19" s="28" t="s">
-        <v>200</v>
-      </c>
       <c r="E19" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F19" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="G19" s="43" t="s">
         <v>183</v>
-      </c>
-      <c r="G19" s="43" t="s">
-        <v>184</v>
       </c>
       <c r="H19" s="25" t="s">
         <v>68</v>
       </c>
       <c r="I19" s="25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J19" s="41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K19" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L19" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M19" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N19"/>
     </row>
@@ -3213,40 +3213,40 @@
         <v>19</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C20" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="E20" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="D20" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>105</v>
-      </c>
       <c r="F20" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="G20" s="43" t="s">
         <v>183</v>
-      </c>
-      <c r="G20" s="43" t="s">
-        <v>184</v>
       </c>
       <c r="H20" s="25" t="s">
         <v>68</v>
       </c>
       <c r="I20" s="25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J20" s="41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K20" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L20" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M20" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N20"/>
     </row>
@@ -3255,40 +3255,40 @@
         <v>20</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C21" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="E21" s="25" t="s">
         <v>106</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>176</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>107</v>
       </c>
       <c r="F21" s="39" t="s">
         <v>4</v>
       </c>
       <c r="G21" s="43" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H21" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="I21" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="J21" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="I21" s="25" t="s">
-        <v>203</v>
-      </c>
-      <c r="J21" s="40" t="s">
-        <v>109</v>
-      </c>
       <c r="K21" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="L21" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="L21" s="34" t="s">
-        <v>178</v>
-      </c>
       <c r="M21" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N21"/>
     </row>
@@ -3297,40 +3297,40 @@
         <v>21</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F22" s="39" t="s">
         <v>4</v>
       </c>
       <c r="G22" s="43" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H22" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I22" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J22" s="40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K22" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="L22" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="L22" s="34" t="s">
-        <v>178</v>
-      </c>
       <c r="M22" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N22"/>
     </row>
@@ -3339,40 +3339,40 @@
         <v>22</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C23" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="E23" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="D23" s="28" t="s">
-        <v>180</v>
-      </c>
-      <c r="E23" s="25" t="s">
-        <v>113</v>
-      </c>
       <c r="F23" s="36" t="s">
+        <v>213</v>
+      </c>
+      <c r="G23" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="H23" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="I23" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="J23" s="42" t="s">
         <v>214</v>
       </c>
-      <c r="G23" s="43" t="s">
-        <v>184</v>
-      </c>
-      <c r="H23" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="I23" s="35" t="s">
-        <v>205</v>
-      </c>
-      <c r="J23" s="42" t="s">
-        <v>215</v>
-      </c>
       <c r="K23" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L23" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M23" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N23"/>
     </row>
@@ -3381,40 +3381,40 @@
         <v>23</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C24" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="E24" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="D24" s="28" t="s">
-        <v>181</v>
-      </c>
-      <c r="E24" s="25" t="s">
-        <v>115</v>
-      </c>
       <c r="F24" s="35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G24" s="43" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I24" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J24" s="42" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K24" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="L24" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="L24" s="34" t="s">
+      <c r="M24" s="38" t="s">
         <v>154</v>
-      </c>
-      <c r="M24" s="38" t="s">
-        <v>155</v>
       </c>
       <c r="N24"/>
     </row>

</xml_diff>

<commit_message>
NHOP Ticket mail send    04/27/21 Ashish
</commit_message>
<xml_diff>
--- a/Configration/GEP_Bot_Configuration_File.xlsx
+++ b/Configration/GEP_Bot_Configuration_File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gep1-my.sharepoint.com/personal/allen_richy_gep_com/Documents/GEP Automation/Configration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashish_jadhav\Documents\UiPath\GEP_Manageengine\Configration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="169" documentId="13_ncr:1_{6EA17F22-868C-46CD-8BBC-388BA0C82BDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E1398FE4-1AA1-445B-970F-52FE9A5463CE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3EABDB-3A41-4E89-9A04-94A117E9C0A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_SPOC_NHOP_Confirmation" sheetId="1" r:id="rId1"/>
@@ -1569,9 +1569,9 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="23.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -1612,7 +1612,7 @@
       </c>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>2</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>9</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>0.22916666666666666</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>0.10416666666666667</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>10</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>10</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>10</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>10</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>10</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
         <v>10</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>19</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>19</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>0.20833333333333334</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
         <v>19</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>0.22916666666666666</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>23</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>23</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>23</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>23</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>23</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>23</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>23</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>23</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>23</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>23</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>23</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>23</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>23</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>23</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>23</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
         <v>23</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>40</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
         <v>40</v>
       </c>
@@ -2309,12 +2309,12 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>56</v>
       </c>
@@ -2322,12 +2322,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>116</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>117</v>
       </c>
@@ -2343,32 +2343,32 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>123</v>
       </c>
@@ -2382,31 +2382,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F323925-C95A-4104-A479-BD78924E652C}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.36328125" style="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.90625" style="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.6328125" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" style="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="96.08984375" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7265625" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="96.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" style="29" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="45" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.54296875" style="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="76.54296875" style="29" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="255.6328125" style="29" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="38.90625" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="76.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="255.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="38.85546875" style="29" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="127" style="29" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="126.453125" style="29" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="84.26953125" style="29" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="24.26953125" style="29"/>
+    <col min="13" max="13" width="126.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="84.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="24.28515625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>58</v>
       </c>
@@ -2448,7 +2448,7 @@
       </c>
       <c r="N1"/>
     </row>
-    <row r="2" spans="1:14" ht="116" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="28">
         <v>1</v>
       </c>
@@ -2490,7 +2490,7 @@
       </c>
       <c r="N2"/>
     </row>
-    <row r="3" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="25">
         <v>2</v>
       </c>
@@ -2532,7 +2532,7 @@
       </c>
       <c r="N3"/>
     </row>
-    <row r="4" spans="1:14" ht="145" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="25">
         <v>3</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="25">
         <v>4</v>
       </c>
@@ -2618,7 +2618,7 @@
       </c>
       <c r="N5"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="25">
         <v>5</v>
       </c>
@@ -2660,7 +2660,7 @@
       </c>
       <c r="N6"/>
     </row>
-    <row r="7" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="25">
         <v>6</v>
       </c>
@@ -2702,7 +2702,7 @@
       </c>
       <c r="N7"/>
     </row>
-    <row r="8" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="25">
         <v>7</v>
       </c>
@@ -2744,7 +2744,7 @@
       </c>
       <c r="N8"/>
     </row>
-    <row r="9" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="25">
         <v>8</v>
       </c>
@@ -2786,7 +2786,7 @@
       </c>
       <c r="N9"/>
     </row>
-    <row r="10" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -2828,7 +2828,7 @@
       </c>
       <c r="N10"/>
     </row>
-    <row r="11" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -2870,7 +2870,7 @@
       </c>
       <c r="N11"/>
     </row>
-    <row r="12" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -2912,7 +2912,7 @@
       </c>
       <c r="N12"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="25">
         <v>12</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="25">
         <v>13</v>
       </c>
@@ -2998,7 +2998,7 @@
       </c>
       <c r="N14"/>
     </row>
-    <row r="15" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="25">
         <v>14</v>
       </c>
@@ -3040,7 +3040,7 @@
       </c>
       <c r="N15"/>
     </row>
-    <row r="16" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="25">
         <v>15</v>
       </c>
@@ -3082,7 +3082,7 @@
       </c>
       <c r="N16"/>
     </row>
-    <row r="17" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="25">
         <v>16</v>
       </c>
@@ -3124,7 +3124,7 @@
       </c>
       <c r="N17"/>
     </row>
-    <row r="18" spans="1:14" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="25">
         <v>17</v>
       </c>
@@ -3166,7 +3166,7 @@
       </c>
       <c r="N18"/>
     </row>
-    <row r="19" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="25">
         <v>18</v>
       </c>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="N19"/>
     </row>
-    <row r="20" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="25">
         <v>19</v>
       </c>
@@ -3250,7 +3250,7 @@
       </c>
       <c r="N20"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="25">
         <v>20</v>
       </c>
@@ -3292,7 +3292,7 @@
       </c>
       <c r="N21"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="25">
         <v>21</v>
       </c>
@@ -3334,7 +3334,7 @@
       </c>
       <c r="N22"/>
     </row>
-    <row r="23" spans="1:14" ht="174" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" ht="180" x14ac:dyDescent="0.25">
       <c r="A23" s="25">
         <v>22</v>
       </c>
@@ -3376,7 +3376,7 @@
       </c>
       <c r="N23"/>
     </row>
-    <row r="24" spans="1:14" ht="203" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" ht="210" x14ac:dyDescent="0.25">
       <c r="A24" s="25">
         <v>23</v>
       </c>

</xml_diff>